<commit_message>
Fix: Formato de hora y lista de eventos en pantalla asistencia.
</commit_message>
<xml_diff>
--- a/DotechRewards/Content/Listas/Actividades_extra_Hallowen.xlsx
+++ b/DotechRewards/Content/Listas/Actividades_extra_Hallowen.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Nombre actividad/evento</t>
   </si>
@@ -41,18 +41,6 @@
     <t>Usuario</t>
   </si>
   <si>
-    <t>miguel.carreon</t>
-  </si>
-  <si>
-    <t>miguelito.nuevo</t>
-  </si>
-  <si>
-    <t>miguel.arista</t>
-  </si>
-  <si>
-    <t>Reventar a eric</t>
-  </si>
-  <si>
     <t>Junta con el gato</t>
   </si>
   <si>
@@ -60,25 +48,25 @@
   </si>
   <si>
     <t>Curso excel</t>
+  </si>
+  <si>
+    <t>raul.gomez</t>
+  </si>
+  <si>
+    <t>Presentacion 28</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF212529"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -104,7 +92,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,7 +376,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,13 +401,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1">
-        <v>43887</v>
+        <v>43157</v>
       </c>
       <c r="D2">
         <v>40</v>
@@ -427,10 +415,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
       </c>
       <c r="C3" s="1">
         <v>43886</v>
@@ -439,31 +427,31 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
       </c>
       <c r="C4" s="1">
         <v>43860</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
       </c>
       <c r="C5" s="1">
         <v>43129</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>120</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix: pre presentación 03-marzo
</commit_message>
<xml_diff>
--- a/DotechRewards/Content/Listas/Actividades_extra_Hallowen.xlsx
+++ b/DotechRewards/Content/Listas/Actividades_extra_Hallowen.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Nombre actividad/evento</t>
   </si>
@@ -41,32 +41,35 @@
     <t>Usuario</t>
   </si>
   <si>
-    <t>Junta con el gato</t>
-  </si>
-  <si>
-    <t>Curso Scrum</t>
-  </si>
-  <si>
-    <t>Curso excel</t>
-  </si>
-  <si>
-    <t>raul.gomez</t>
-  </si>
-  <si>
-    <t>Presentacion 28</t>
+    <t>karen.arceo</t>
+  </si>
+  <si>
+    <t>Cumpleaños 2019</t>
+  </si>
+  <si>
+    <t>Cumpleaños 2020</t>
+  </si>
+  <si>
+    <t>1er aniversario Dotech</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -89,10 +92,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,7 +380,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,61 +403,52 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
+    <row r="2" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1">
-        <v>43157</v>
+        <v>43466</v>
       </c>
       <c r="D2">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
+    <row r="3" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1">
-        <v>43886</v>
+        <v>43831</v>
       </c>
       <c r="D3">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
       <c r="C4" s="1">
-        <v>43860</v>
+        <v>43893</v>
       </c>
       <c r="D4" s="2">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1">
-        <v>43129</v>
-      </c>
-      <c r="D5" s="2">
-        <v>120</v>
-      </c>
+    <row r="5" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:D3"/>

</xml_diff>

<commit_message>
Fix: enlaces a descargar de lista de asistencia, liga para recuperar contrasñea
</commit_message>
<xml_diff>
--- a/DotechRewards/Content/Listas/Actividades_extra_Hallowen.xlsx
+++ b/DotechRewards/Content/Listas/Actividades_extra_Hallowen.xlsx
@@ -41,9 +41,6 @@
     <t>Usuario</t>
   </si>
   <si>
-    <t>karen.arceo</t>
-  </si>
-  <si>
     <t>Cumpleaños 2019</t>
   </si>
   <si>
@@ -51,6 +48,9 @@
   </si>
   <si>
     <t>1er aniversario Dotech</t>
+  </si>
+  <si>
+    <t>adolfo.cardenas</t>
   </si>
 </sst>
 </file>
@@ -380,7 +380,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,10 +405,10 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
       </c>
       <c r="C2" s="1">
         <v>43466</v>
@@ -419,10 +419,10 @@
     </row>
     <row r="3" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1">
         <v>43831</v>
@@ -433,10 +433,10 @@
     </row>
     <row r="4" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1">
         <v>43893</v>

</xml_diff>